<commit_message>
update routing in progress
</commit_message>
<xml_diff>
--- a/notes/android_nci_notes.xlsx
+++ b/notes/android_nci_notes.xlsx
@@ -9,19 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2604" windowWidth="23040" windowHeight="8532" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4464" windowWidth="23040" windowHeight="8532" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="tNFC_CB" sheetId="11" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="doInit" sheetId="1" r:id="rId2"/>
     <sheet name="LLCP" sheetId="10" r:id="rId3"/>
     <sheet name="hal-tml" sheetId="6" r:id="rId4"/>
     <sheet name="Threads" sheetId="7" r:id="rId5"/>
     <sheet name="fw dnld" sheetId="5" r:id="rId6"/>
     <sheet name="callbacks" sheetId="2" r:id="rId7"/>
     <sheet name="NCI" sheetId="3" r:id="rId8"/>
-    <sheet name="Java Layer" sheetId="4" r:id="rId9"/>
+    <sheet name="MBOX" sheetId="4" r:id="rId9"/>
     <sheet name="setDefaultRoute" sheetId="8" r:id="rId10"/>
+    <sheet name="GKI" sheetId="12" r:id="rId11"/>
+    <sheet name="CardEmu" sheetId="13" r:id="rId12"/>
+    <sheet name="Routing" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -210,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="412">
   <si>
     <t>NativeNfcManager.cpp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1559,6 +1562,252 @@
   <si>
     <t>/* event == NFC_ERROR_CEVT */</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NfcAdaptation::Initialize</t>
+  </si>
+  <si>
+    <t>GKI_run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GKI_create_task(NFCA_TASK, BTU_TASK, "NFCA_TASK", ..)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GKI_create_task(Thread, MMI_TASK, "NFCA_THREAD", ..)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GKI_create_task(nfc_task, NFC_TASK, "NFC_TASK", …)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pthread_create( &amp;timer_thread_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              &amp;timer_attr,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              timer_thread,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              NULL)</t>
+  </si>
+  <si>
+    <t>GKI_timer_update( 1 );</t>
+  </si>
+  <si>
+    <t>while(!shutdown_timer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        delay.tv_sec = timeout / 1000;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        delay.tv_nsec = 1000 * 1000 * (timeout%1000);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        /* [u]sleep can't be used because it uses SIGALRM */</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            err = nanosleep(&amp;delay, &amp;delay);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        } while (err &lt; 0 &amp;&amp; errno ==EINTR);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GKI_timer_update(1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>/* Process all incoming NCI messages */</t>
+  </si>
+  <si>
+    <t>while ((p_msg = (BT_HDR *) GKI_read_mbox (NFC_MBOX_ID)) != NULL)</t>
+  </si>
+  <si>
+    <t>if (event &amp; NFC_MBOX_EVT_MASK)</t>
+  </si>
+  <si>
+    <t>/* Process gki timer tick */</t>
+  </si>
+  <si>
+    <t>if (event &amp; NFC_TIMER_EVT_MASK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/* Process quick timer tick */</t>
+  </si>
+  <si>
+    <t>if (event &amp; NFC_QUICK_TIMER_EVT_MASK)</t>
+  </si>
+  <si>
+    <t>if (event &amp; NFA_MBOX_EVT_MASK)</t>
+  </si>
+  <si>
+    <t>while ((p_msg = (BT_HDR *) GKI_read_mbox (NFA_MBOX_ID)) != NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                nfa_sys_event (p_msg);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t>if (event &amp; NFA_TIMER_EVT_MASK)</t>
+  </si>
+  <si>
+    <t>nfa_sys_timer_update</t>
+  </si>
+  <si>
+    <t>nfa_ce_action_tbl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE_SetActivatedTagType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ce_select_t4t</t>
+  </si>
+  <si>
+    <t>nfa_ce_discovery_cback</t>
+  </si>
+  <si>
+    <t>NFA_CE_API_REG_LISTEN_EVT</t>
+  </si>
+  <si>
+    <t>nfc_ce_api.c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFA_CeConfigureUiccListenTech</t>
+  </si>
+  <si>
+    <t>NFA_CeConfigureEseListenTech</t>
+  </si>
+  <si>
+    <t>NFA_CeRegisterFelicaSystemCodeOnDH</t>
+  </si>
+  <si>
+    <t>NFA_CeDeregisterFelicaSystemCodeOnDH</t>
+  </si>
+  <si>
+    <t>NFA_CeDeregisterAidOnDH</t>
+  </si>
+  <si>
+    <t>NFA_CeSetIsoDepListenTech</t>
+  </si>
+  <si>
+    <t>nfa_ce_api_reg_listen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nfa_ce_start_listening</t>
+  </si>
+  <si>
+    <t>disc_handle = nfa_dm_add_rf_discover (listen_mask, NFA_DM_DISC_HOST_ID_DH, nfa_ce_discovery_cback);</t>
+  </si>
+  <si>
+    <t>ce_msg.activate_ntf.hdr.event = NFA_CE_ACTIVATE_NTF_EVT;</t>
+  </si>
+  <si>
+    <t>ce_msg.activate_ntf.p_activation_params = &amp;p_data-&gt;activate;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nfa_ce_hdl_event ((void *) &amp;ce_msg);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/* card activated */</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nfa_ce_activate_ntf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nfa_dm_excl_disc_cback</t>
+  </si>
+  <si>
+    <t>nfa_dm_cb.disc_cb.excl_disc_entry.p_disc_cback        = p_disc_cback;</t>
+  </si>
+  <si>
+    <t>nfa_dm_start_excl_discovery</t>
+  </si>
+  <si>
+    <t>/* nfa_dm_excl_disc_cback */</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nfa_dm_disc_notify_activation</t>
+  </si>
+  <si>
+    <t>(*(nfa_dm_cb.disc_cb.excl_disc_entry.p_disc_cback)) (NFA_DM_RF_DISC_ACTIVATED_EVT, p_data);</t>
+  </si>
+  <si>
+    <t>GKI_send_msg (NFC_TASK, NFC_MBOX_ID, p_msg);</t>
+  </si>
+  <si>
+    <t>GKI_send_event</t>
+  </si>
+  <si>
+    <t>pthread_cond_signal</t>
+  </si>
+  <si>
+    <t>pthread_cond_timedwait</t>
+  </si>
+  <si>
+    <t>mbox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>while (TRUE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>event = GKI_wait (0xFFFF, 0);</t>
+  </si>
+  <si>
+    <t>NfcService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applyRouting</t>
+  </si>
+  <si>
+    <t>enableInternal</t>
+  </si>
+  <si>
+    <t>computeDiscoveryParameters</t>
+  </si>
+  <si>
+    <t>nfcManager_setDefaultRoute</t>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoutingManager::getInstance().setDefaultRoute(defaultRouteEntry, defaultProtoRouteEntry, defaultTechRouteEntry);</t>
+  </si>
+  <si>
+    <t>RoutingManager::getInstance().commitRouting();</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1899,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1766,13 +2015,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1799,9 +2074,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1844,6 +2116,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2229,6 +2513,439 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Curved Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4907280" y="274320"/>
+          <a:ext cx="1752600" cy="358140"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Curved Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2411730" y="986790"/>
+          <a:ext cx="350520" cy="220980"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Curved Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3745230" y="1725930"/>
+          <a:ext cx="350520" cy="220980"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Curved Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9944100" y="487680"/>
+          <a:ext cx="982980" cy="563880"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Curved Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7239000" y="2613660"/>
+          <a:ext cx="6088380" cy="2049780"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Curved Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="11071860" y="4328160"/>
+          <a:ext cx="1341120" cy="1287780"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Curved Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="9258300" y="4975860"/>
+          <a:ext cx="1013460" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Curved Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1344930" y="1626870"/>
+          <a:ext cx="434340" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Curved Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4457700" y="3566160"/>
+          <a:ext cx="3383280" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2509,270 +3226,270 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="13"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="12"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="16"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="15"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>197</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="16"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="15"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="16"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="15"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>199</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="O7" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="16"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="15"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>179</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="16"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="15"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>180</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="16"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="15"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>181</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="16"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="15"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>182</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="16"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="15"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>200</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="16"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="15"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>201</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O13" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="16"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="15"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="16"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="15"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="O15" s="14" t="s">
+      <c r="O15" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="16"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="15"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>203</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="16"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="15"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>204</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="16"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="15"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>205</v>
       </c>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="19"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="18"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2978,243 +3695,243 @@
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="O65" s="11" t="s">
+      <c r="O65" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P65" s="12"/>
-      <c r="Q65" s="12"/>
-      <c r="R65" s="12"/>
-      <c r="S65" s="12"/>
-      <c r="T65" s="12"/>
-      <c r="U65" s="12"/>
-      <c r="V65" s="12"/>
-      <c r="W65" s="13"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="11"/>
+      <c r="U65" s="11"/>
+      <c r="V65" s="11"/>
+      <c r="W65" s="12"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>238</v>
       </c>
-      <c r="O66" s="14" t="s">
+      <c r="O66" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="16"/>
+      <c r="P66" s="14"/>
+      <c r="Q66" s="14"/>
+      <c r="R66" s="14"/>
+      <c r="S66" s="14"/>
+      <c r="T66" s="14"/>
+      <c r="U66" s="14"/>
+      <c r="V66" s="14"/>
+      <c r="W66" s="15"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O67" s="14" t="s">
+      <c r="O67" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-      <c r="U67" s="21" t="s">
+      <c r="P67" s="14"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="V67" s="15"/>
-      <c r="W67" s="16"/>
+      <c r="V67" s="14"/>
+      <c r="W67" s="15"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>184</v>
       </c>
-      <c r="O68" s="14" t="s">
+      <c r="O68" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="22" t="s">
+      <c r="P68" s="14"/>
+      <c r="Q68" s="14"/>
+      <c r="R68" s="14"/>
+      <c r="S68" s="14"/>
+      <c r="T68" s="14"/>
+      <c r="U68" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="V68" s="15"/>
-      <c r="W68" s="16"/>
+      <c r="V68" s="14"/>
+      <c r="W68" s="15"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O69" s="14" t="s">
+      <c r="O69" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="22" t="s">
+      <c r="P69" s="14"/>
+      <c r="Q69" s="14"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="14"/>
+      <c r="T69" s="14"/>
+      <c r="U69" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="V69" s="15"/>
-      <c r="W69" s="16"/>
+      <c r="V69" s="14"/>
+      <c r="W69" s="15"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O70" s="14" t="s">
+      <c r="O70" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="15"/>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-      <c r="U70" s="22" t="s">
+      <c r="P70" s="14"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="V70" s="15"/>
-      <c r="W70" s="16"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="15"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O71" s="14" t="s">
+      <c r="O71" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="P71" s="15"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="22" t="s">
+      <c r="P71" s="14"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+      <c r="U71" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="V71" s="15"/>
-      <c r="W71" s="16"/>
+      <c r="V71" s="14"/>
+      <c r="W71" s="15"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O72" s="14" t="s">
+      <c r="O72" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="P72" s="15"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
-      <c r="U72" s="22" t="s">
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+      <c r="U72" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="V72" s="15"/>
-      <c r="W72" s="16"/>
+      <c r="V72" s="14"/>
+      <c r="W72" s="15"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O73" s="14" t="s">
+      <c r="O73" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="P73" s="15"/>
-      <c r="Q73" s="15"/>
-      <c r="R73" s="15"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="15"/>
-      <c r="U73" s="22"/>
-      <c r="V73" s="15"/>
-      <c r="W73" s="16"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+      <c r="U73" s="21"/>
+      <c r="V73" s="14"/>
+      <c r="W73" s="15"/>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O74" s="14" t="s">
+      <c r="O74" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="P74" s="15"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="22" t="s">
+      <c r="P74" s="14"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
+      <c r="U74" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="V74" s="15"/>
-      <c r="W74" s="16"/>
+      <c r="V74" s="14"/>
+      <c r="W74" s="15"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O75" s="14" t="s">
+      <c r="O75" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="22"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="16"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="14"/>
+      <c r="R75" s="14"/>
+      <c r="S75" s="14"/>
+      <c r="T75" s="14"/>
+      <c r="U75" s="21"/>
+      <c r="V75" s="14"/>
+      <c r="W75" s="15"/>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O76" s="14" t="s">
+      <c r="O76" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="P76" s="15"/>
-      <c r="Q76" s="15"/>
-      <c r="R76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="15"/>
-      <c r="U76" s="22" t="s">
+      <c r="P76" s="14"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="14"/>
+      <c r="S76" s="14"/>
+      <c r="T76" s="14"/>
+      <c r="U76" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="V76" s="15"/>
-      <c r="W76" s="16"/>
+      <c r="V76" s="14"/>
+      <c r="W76" s="15"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O77" s="14" t="s">
+      <c r="O77" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="15"/>
-      <c r="U77" s="22" t="s">
+      <c r="P77" s="14"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="14"/>
+      <c r="S77" s="14"/>
+      <c r="T77" s="14"/>
+      <c r="U77" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="V77" s="15"/>
-      <c r="W77" s="16"/>
+      <c r="V77" s="14"/>
+      <c r="W77" s="15"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O78" s="14" t="s">
+      <c r="O78" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="22" t="s">
+      <c r="P78" s="14"/>
+      <c r="Q78" s="14"/>
+      <c r="R78" s="14"/>
+      <c r="S78" s="14"/>
+      <c r="T78" s="14"/>
+      <c r="U78" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="V78" s="15"/>
-      <c r="W78" s="16"/>
+      <c r="V78" s="14"/>
+      <c r="W78" s="15"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O79" s="14" t="s">
+      <c r="O79" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
-      <c r="R79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="15"/>
-      <c r="U79" s="22" t="s">
+      <c r="P79" s="14"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="14"/>
+      <c r="S79" s="14"/>
+      <c r="T79" s="14"/>
+      <c r="U79" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="V79" s="15"/>
-      <c r="W79" s="16"/>
+      <c r="V79" s="14"/>
+      <c r="W79" s="15"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O80" s="17" t="s">
+      <c r="O80" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="18"/>
-      <c r="R80" s="18"/>
-      <c r="S80" s="18"/>
-      <c r="T80" s="18"/>
-      <c r="U80" s="18"/>
-      <c r="V80" s="18"/>
-      <c r="W80" s="19"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="17"/>
+      <c r="R80" s="17"/>
+      <c r="S80" s="17"/>
+      <c r="T80" s="17"/>
+      <c r="U80" s="17"/>
+      <c r="V80" s="17"/>
+      <c r="W80" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3362,6 +4079,429 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:W33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="M3" t="s">
+        <v>337</v>
+      </c>
+      <c r="S3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" t="s">
+        <v>341</v>
+      </c>
+      <c r="T4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>339</v>
+      </c>
+      <c r="N5" t="s">
+        <v>342</v>
+      </c>
+      <c r="T5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>343</v>
+      </c>
+      <c r="T6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>344</v>
+      </c>
+      <c r="T7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>340</v>
+      </c>
+      <c r="T9" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>115</v>
+      </c>
+      <c r="T12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>402</v>
+      </c>
+      <c r="T13" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>403</v>
+      </c>
+      <c r="T14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>357</v>
+      </c>
+      <c r="T16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>359</v>
+      </c>
+      <c r="T17" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="18" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="23" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>362</v>
+      </c>
+      <c r="T23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>363</v>
+      </c>
+      <c r="U24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>364</v>
+      </c>
+      <c r="W26" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="27" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="28" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="29" spans="9:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="30" spans="9:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>368</v>
+      </c>
+      <c r="R30" s="23" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>369</v>
+      </c>
+      <c r="R31" s="24"/>
+    </row>
+    <row r="32" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>370</v>
+      </c>
+      <c r="R32" s="24"/>
+    </row>
+    <row r="33" spans="18:18" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="25"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>374</v>
+      </c>
+      <c r="M19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>386</v>
+      </c>
+      <c r="N20" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>387</v>
+      </c>
+      <c r="O21" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>388</v>
+      </c>
+      <c r="P22" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>392</v>
+      </c>
+      <c r="L28" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>391</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E17"/>
@@ -3385,10 +4525,10 @@
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3475,8 +4615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3502,7 +4642,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3557,7 +4697,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3587,7 +4727,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3696,7 +4836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -4067,8 +5207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V66"/>
   <sheetViews>
-    <sheetView topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4297,7 +5437,7 @@
       <c r="Q49" t="s">
         <v>264</v>
       </c>
-      <c r="R49" s="10" t="s">
+      <c r="R49" s="9" t="s">
         <v>263</v>
       </c>
       <c r="V49" t="s">
@@ -4308,7 +5448,7 @@
       <c r="B50" t="s">
         <v>261</v>
       </c>
-      <c r="R50" s="20" t="s">
+      <c r="R50" s="19" t="s">
         <v>307</v>
       </c>
       <c r="V50" t="s">
@@ -4400,7 +5540,7 @@
       <c r="B64" t="s">
         <v>298</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="22" t="s">
         <v>308</v>
       </c>
       <c r="D64" t="s">
@@ -4411,24 +5551,24 @@
       <c r="C65" t="s">
         <v>295</v>
       </c>
-      <c r="Q65" s="10" t="s">
+      <c r="Q65" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="S65" s="23" t="s">
+      <c r="S65" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="T65" s="10" t="s">
+      <c r="T65" s="9" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="66" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="Q66" s="20" t="s">
+      <c r="Q66" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="S66" s="23" t="s">
+      <c r="S66" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="T66" s="20" t="s">
+      <c r="T66" s="19" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4445,7 +5585,7 @@
   <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4489,8 +5629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>